<commit_message>
Add address schema and mandatory fields
</commit_message>
<xml_diff>
--- a/api-hub-example/example.xlsx
+++ b/api-hub-example/example.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/areddy/Downloads/employee-management-service/api-hub-example/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57EC36BB-3F25-F14E-AB34-CEFF7E97162E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0D3D7D9-D4DE-274D-A61C-BE332A9D9E20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="660" windowWidth="30240" windowHeight="17840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="56">
   <si>
     <t>Category</t>
   </si>
@@ -117,9 +117,6 @@
     <t>address</t>
   </si>
   <si>
-    <t>country</t>
-  </si>
-  <si>
     <t>String</t>
   </si>
   <si>
@@ -169,6 +166,30 @@
   </si>
   <si>
     <t>/employee</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>line1</t>
+  </si>
+  <si>
+    <t>line2</t>
+  </si>
+  <si>
+    <t>city</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>Zip</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>dto</t>
   </si>
 </sst>
 </file>
@@ -225,7 +246,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -256,8 +277,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -280,6 +307,34 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -296,7 +351,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -348,6 +403,22 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="API organization (organization)LockedColumnStyle" xfId="1" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
@@ -671,7 +742,7 @@
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:F5"/>
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" customHeight="1"/>
@@ -765,7 +836,7 @@
   <dimension ref="A1:N31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12:O12"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" customHeight="1"/>
@@ -833,7 +904,7 @@
         <v>24</v>
       </c>
       <c r="K2" s="27" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="L2" s="12" t="s">
         <v>25</v>
@@ -869,7 +940,9 @@
       <c r="C4" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="D4" s="4"/>
+      <c r="D4" s="4" t="s">
+        <v>48</v>
+      </c>
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
       <c r="G4" s="13"/>
@@ -887,9 +960,11 @@
         <v>30</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="D5" s="4"/>
+        <v>30</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>48</v>
+      </c>
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
       <c r="G5" s="13"/>
@@ -904,10 +979,10 @@
     <row r="6" spans="1:14" ht="17" customHeight="1">
       <c r="A6" s="5"/>
       <c r="B6" s="14" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
@@ -923,12 +998,8 @@
     </row>
     <row r="7" spans="1:14" ht="17" customHeight="1">
       <c r="A7" s="5"/>
-      <c r="B7" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="C7" s="14" t="s">
-        <v>34</v>
-      </c>
+      <c r="B7" s="14"/>
+      <c r="C7" s="14"/>
       <c r="D7" s="16"/>
       <c r="E7" s="16"/>
       <c r="F7" s="16"/>
@@ -1007,7 +1078,7 @@
     </row>
     <row r="12" spans="1:14" ht="17" customHeight="1">
       <c r="A12" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B12" s="17"/>
       <c r="C12" s="17"/>
@@ -1051,9 +1122,11 @@
         <v>28</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="D14" s="16"/>
+        <v>31</v>
+      </c>
+      <c r="D14" s="14" t="s">
+        <v>48</v>
+      </c>
       <c r="E14" s="16"/>
       <c r="F14" s="16"/>
       <c r="G14" s="16"/>
@@ -1068,12 +1141,14 @@
     <row r="15" spans="1:14" ht="15" customHeight="1">
       <c r="A15" s="14"/>
       <c r="B15" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="D15" s="16"/>
+        <v>31</v>
+      </c>
+      <c r="D15" s="14" t="s">
+        <v>48</v>
+      </c>
       <c r="E15" s="16"/>
       <c r="F15" s="16"/>
       <c r="G15" s="16"/>
@@ -1088,12 +1163,14 @@
     <row r="16" spans="1:14" ht="15" customHeight="1">
       <c r="A16" s="14"/>
       <c r="B16" s="14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="D16" s="16"/>
+        <v>31</v>
+      </c>
+      <c r="D16" s="14" t="s">
+        <v>48</v>
+      </c>
       <c r="E16" s="16"/>
       <c r="F16" s="16"/>
       <c r="G16" s="16"/>
@@ -1111,9 +1188,11 @@
         <v>30</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="D17" s="16"/>
+        <v>30</v>
+      </c>
+      <c r="D17" s="14" t="s">
+        <v>48</v>
+      </c>
       <c r="E17" s="16"/>
       <c r="F17" s="16"/>
       <c r="G17" s="16"/>
@@ -1127,12 +1206,8 @@
     </row>
     <row r="18" spans="1:14" ht="15" customHeight="1">
       <c r="A18" s="14"/>
-      <c r="B18" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="C18" s="14" t="s">
-        <v>32</v>
-      </c>
+      <c r="B18" s="14"/>
+      <c r="C18" s="14"/>
       <c r="D18" s="16"/>
       <c r="E18" s="16"/>
       <c r="F18" s="16"/>
@@ -1227,7 +1302,7 @@
     </row>
     <row r="24" spans="1:14" ht="17" customHeight="1">
       <c r="A24" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B24" s="17"/>
       <c r="C24" s="17"/>
@@ -1243,7 +1318,7 @@
         <v>24</v>
       </c>
       <c r="K24" s="27" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="L24" s="12" t="s">
         <v>25</v>
@@ -1279,7 +1354,9 @@
       <c r="C26" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="D26" s="16"/>
+      <c r="D26" s="14" t="s">
+        <v>48</v>
+      </c>
       <c r="E26" s="16"/>
       <c r="F26" s="16"/>
       <c r="G26" s="16"/>
@@ -1294,12 +1371,14 @@
     <row r="27" spans="1:14" ht="15" customHeight="1">
       <c r="A27" s="14"/>
       <c r="B27" s="14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C27" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="D27" s="16"/>
+        <v>34</v>
+      </c>
+      <c r="D27" s="14" t="s">
+        <v>48</v>
+      </c>
       <c r="E27" s="16"/>
       <c r="F27" s="16"/>
       <c r="G27" s="16"/>
@@ -1383,10 +1462,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" customHeight="1"/>
@@ -1433,16 +1512,16 @@
       <c r="E2" s="22"/>
       <c r="F2" s="22"/>
       <c r="G2" s="24" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="18" customHeight="1">
       <c r="A3" s="5"/>
       <c r="B3" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>40</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>41</v>
       </c>
       <c r="D3" s="26"/>
       <c r="E3" s="4"/>
@@ -1452,10 +1531,10 @@
     <row r="4" spans="1:7" ht="18" customHeight="1">
       <c r="A4" s="5"/>
       <c r="B4" s="25" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D4" s="26"/>
       <c r="E4" s="4"/>
@@ -1465,10 +1544,10 @@
     <row r="5" spans="1:7" ht="17" customHeight="1">
       <c r="A5" s="5"/>
       <c r="B5" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D5" s="26"/>
       <c r="E5" s="4"/>
@@ -1478,10 +1557,10 @@
     <row r="6" spans="1:7" ht="17" customHeight="1">
       <c r="A6" s="5"/>
       <c r="B6" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D6" s="26"/>
       <c r="E6" s="4"/>
@@ -1491,10 +1570,10 @@
     <row r="7" spans="1:7" ht="18" customHeight="1">
       <c r="A7" s="5"/>
       <c r="B7" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>45</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>46</v>
       </c>
       <c r="D7" s="26"/>
       <c r="E7" s="4"/>
@@ -1511,40 +1590,105 @@
       <c r="G8" s="25"/>
     </row>
     <row r="9" spans="1:7" ht="17" customHeight="1">
-      <c r="A9" s="5"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="26"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="25"/>
+      <c r="A9" s="35" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" s="36"/>
+      <c r="C9" s="36"/>
+      <c r="D9" s="37"/>
+      <c r="E9" s="36"/>
+      <c r="F9" s="36" t="s">
+        <v>55</v>
+      </c>
+      <c r="G9" s="38"/>
     </row>
     <row r="10" spans="1:7" ht="17" customHeight="1">
       <c r="A10" s="5"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="26"/>
+      <c r="B10" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="26" t="s">
+        <v>48</v>
+      </c>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
       <c r="G10" s="4"/>
     </row>
     <row r="11" spans="1:7" ht="17" customHeight="1">
       <c r="A11" s="5"/>
-      <c r="B11" s="25"/>
-      <c r="C11" s="4"/>
+      <c r="B11" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>31</v>
+      </c>
       <c r="D11" s="26"/>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
     </row>
     <row r="12" spans="1:7" ht="17" customHeight="1">
-      <c r="A12" s="5"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="26"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
+      <c r="A12" s="29"/>
+      <c r="B12" s="30" t="s">
+        <v>51</v>
+      </c>
+      <c r="C12" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" s="31" t="s">
+        <v>48</v>
+      </c>
+      <c r="E12" s="30"/>
+      <c r="F12" s="30"/>
+      <c r="G12" s="30"/>
+    </row>
+    <row r="13" spans="1:7" ht="16" customHeight="1">
+      <c r="A13" s="32"/>
+      <c r="B13" s="33" t="s">
+        <v>52</v>
+      </c>
+      <c r="C13" s="34" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13" s="34" t="s">
+        <v>48</v>
+      </c>
+      <c r="E13" s="32"/>
+      <c r="F13" s="32"/>
+      <c r="G13" s="32"/>
+    </row>
+    <row r="14" spans="1:7" ht="16" customHeight="1">
+      <c r="A14" s="32"/>
+      <c r="B14" s="33" t="s">
+        <v>53</v>
+      </c>
+      <c r="C14" s="34" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" s="34" t="s">
+        <v>48</v>
+      </c>
+      <c r="E14" s="32"/>
+      <c r="F14" s="32"/>
+      <c r="G14" s="32"/>
+    </row>
+    <row r="15" spans="1:7" ht="16" customHeight="1">
+      <c r="A15" s="32"/>
+      <c r="B15" s="33" t="s">
+        <v>54</v>
+      </c>
+      <c r="C15" s="34" t="s">
+        <v>31</v>
+      </c>
+      <c r="D15" s="34" t="s">
+        <v>48</v>
+      </c>
+      <c r="E15" s="32"/>
+      <c r="F15" s="32"/>
+      <c r="G15" s="32"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
RECOVERY: restore all local changes
</commit_message>
<xml_diff>
--- a/api-hub-example/example.xlsx
+++ b/api-hub-example/example.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/areddy/Downloads/employee-management-service/api-hub-example/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57EC36BB-3F25-F14E-AB34-CEFF7E97162E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{370A1FAC-F580-9E46-8CAD-5EE6E7AD699D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="660" windowWidth="30240" windowHeight="17840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="660" windowWidth="30240" windowHeight="18980" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="API organization (organization)" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="57">
   <si>
     <t>Category</t>
   </si>
@@ -169,6 +169,30 @@
   </si>
   <si>
     <t>/employee</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>Reusable address value object</t>
+  </si>
+  <si>
+    <t>line1</t>
+  </si>
+  <si>
+    <t>line2</t>
+  </si>
+  <si>
+    <t>city</t>
+  </si>
+  <si>
+    <t>state</t>
+  </si>
+  <si>
+    <t>pincode</t>
+  </si>
+  <si>
+    <t>DTO</t>
   </si>
 </sst>
 </file>
@@ -257,7 +281,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -280,6 +304,34 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -296,7 +348,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -348,6 +400,15 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="API organization (organization)LockedColumnStyle" xfId="1" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
@@ -670,8 +731,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:F5"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" customHeight="1"/>
@@ -764,8 +825,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12:O12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" customHeight="1"/>
@@ -869,7 +930,9 @@
       <c r="C4" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="D4" s="4"/>
+      <c r="D4" s="4" t="s">
+        <v>49</v>
+      </c>
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
       <c r="G4" s="13"/>
@@ -887,9 +950,11 @@
         <v>30</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="D5" s="4"/>
+        <v>30</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>49</v>
+      </c>
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
       <c r="G5" s="13"/>
@@ -904,12 +969,14 @@
     <row r="6" spans="1:14" ht="17" customHeight="1">
       <c r="A6" s="5"/>
       <c r="B6" s="14" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="D6" s="4"/>
+        <v>34</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>49</v>
+      </c>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
       <c r="G6" s="13"/>
@@ -923,13 +990,9 @@
     </row>
     <row r="7" spans="1:14" ht="17" customHeight="1">
       <c r="A7" s="5"/>
-      <c r="B7" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="C7" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="D7" s="16"/>
+      <c r="B7" s="14"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
       <c r="E7" s="16"/>
       <c r="F7" s="16"/>
       <c r="G7" s="13"/>
@@ -1010,7 +1073,9 @@
         <v>35</v>
       </c>
       <c r="B12" s="17"/>
-      <c r="C12" s="17"/>
+      <c r="C12" s="17" t="s">
+        <v>22</v>
+      </c>
       <c r="D12" s="18"/>
       <c r="E12" s="18"/>
       <c r="F12" s="10" t="s">
@@ -1033,7 +1098,7 @@
       <c r="C13" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="D13" s="16"/>
+      <c r="D13" s="14"/>
       <c r="E13" s="16"/>
       <c r="F13" s="16"/>
       <c r="G13" s="16"/>
@@ -1053,7 +1118,9 @@
       <c r="C14" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="D14" s="16"/>
+      <c r="D14" s="14" t="s">
+        <v>49</v>
+      </c>
       <c r="E14" s="16"/>
       <c r="F14" s="16"/>
       <c r="G14" s="16"/>
@@ -1073,7 +1140,9 @@
       <c r="C15" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="D15" s="16"/>
+      <c r="D15" s="14" t="s">
+        <v>49</v>
+      </c>
       <c r="E15" s="16"/>
       <c r="F15" s="16"/>
       <c r="G15" s="16"/>
@@ -1093,7 +1162,9 @@
       <c r="C16" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="D16" s="16"/>
+      <c r="D16" s="14" t="s">
+        <v>49</v>
+      </c>
       <c r="E16" s="16"/>
       <c r="F16" s="16"/>
       <c r="G16" s="16"/>
@@ -1111,10 +1182,12 @@
         <v>30</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="D17" s="16"/>
-      <c r="E17" s="16"/>
+        <v>30</v>
+      </c>
+      <c r="D17" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="E17" s="8"/>
       <c r="F17" s="16"/>
       <c r="G17" s="16"/>
       <c r="H17" s="16"/>
@@ -1127,12 +1200,8 @@
     </row>
     <row r="18" spans="1:14" ht="15" customHeight="1">
       <c r="A18" s="14"/>
-      <c r="B18" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="C18" s="14" t="s">
-        <v>32</v>
-      </c>
+      <c r="B18" s="14"/>
+      <c r="C18" s="14"/>
       <c r="D18" s="16"/>
       <c r="E18" s="16"/>
       <c r="F18" s="16"/>
@@ -1230,7 +1299,9 @@
         <v>38</v>
       </c>
       <c r="B24" s="17"/>
-      <c r="C24" s="17"/>
+      <c r="C24" s="17" t="s">
+        <v>22</v>
+      </c>
       <c r="D24" s="18"/>
       <c r="E24" s="18"/>
       <c r="F24" s="10" t="s">
@@ -1259,7 +1330,7 @@
       <c r="C25" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="D25" s="16"/>
+      <c r="D25" s="14"/>
       <c r="E25" s="16"/>
       <c r="F25" s="16"/>
       <c r="G25" s="16"/>
@@ -1279,7 +1350,9 @@
       <c r="C26" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="D26" s="16"/>
+      <c r="D26" s="14" t="s">
+        <v>49</v>
+      </c>
       <c r="E26" s="16"/>
       <c r="F26" s="16"/>
       <c r="G26" s="16"/>
@@ -1299,7 +1372,9 @@
       <c r="C27" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="D27" s="16"/>
+      <c r="D27" s="14" t="s">
+        <v>49</v>
+      </c>
       <c r="E27" s="16"/>
       <c r="F27" s="16"/>
       <c r="G27" s="16"/>
@@ -1383,10 +1458,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" customHeight="1"/>
@@ -1520,31 +1595,125 @@
       <c r="G9" s="25"/>
     </row>
     <row r="10" spans="1:7" ht="17" customHeight="1">
-      <c r="A10" s="5"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="26"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
+      <c r="A10" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" s="22"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="23"/>
+      <c r="E10" s="22"/>
+      <c r="F10" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="G10" s="24" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="11" spans="1:7" ht="17" customHeight="1">
       <c r="A11" s="5"/>
-      <c r="B11" s="25"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="26"/>
+      <c r="B11" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" s="26" t="s">
+        <v>49</v>
+      </c>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
     </row>
     <row r="12" spans="1:7" ht="17" customHeight="1">
-      <c r="A12" s="5"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="26"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
+      <c r="A12" s="29"/>
+      <c r="B12" s="30" t="s">
+        <v>52</v>
+      </c>
+      <c r="C12" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" s="31"/>
+      <c r="E12" s="30"/>
+      <c r="F12" s="30"/>
+      <c r="G12" s="30"/>
+    </row>
+    <row r="13" spans="1:7" ht="16" customHeight="1">
+      <c r="A13" s="32"/>
+      <c r="B13" s="34" t="s">
+        <v>53</v>
+      </c>
+      <c r="C13" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" s="34" t="s">
+        <v>49</v>
+      </c>
+      <c r="E13" s="32"/>
+      <c r="F13" s="32"/>
+      <c r="G13" s="32"/>
+    </row>
+    <row r="14" spans="1:7" ht="16" customHeight="1">
+      <c r="A14" s="32"/>
+      <c r="B14" s="34" t="s">
+        <v>54</v>
+      </c>
+      <c r="C14" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="D14" s="34" t="s">
+        <v>49</v>
+      </c>
+      <c r="E14" s="32"/>
+      <c r="F14" s="32"/>
+      <c r="G14" s="32"/>
+    </row>
+    <row r="15" spans="1:7" ht="16" customHeight="1">
+      <c r="A15" s="32"/>
+      <c r="B15" s="34" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="D15" s="34" t="s">
+        <v>49</v>
+      </c>
+      <c r="E15" s="32"/>
+      <c r="F15" s="32"/>
+      <c r="G15" s="32"/>
+    </row>
+    <row r="16" spans="1:7" ht="16" customHeight="1">
+      <c r="A16" s="32"/>
+      <c r="B16" s="35" t="s">
+        <v>55</v>
+      </c>
+      <c r="C16" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="D16" s="35" t="s">
+        <v>49</v>
+      </c>
+      <c r="E16" s="32"/>
+      <c r="F16" s="32"/>
+      <c r="G16" s="32"/>
+    </row>
+    <row r="17" spans="1:7" ht="16" customHeight="1">
+      <c r="A17" s="32"/>
+      <c r="B17" s="32"/>
+      <c r="C17" s="32"/>
+      <c r="D17" s="32"/>
+      <c r="E17" s="32"/>
+      <c r="F17" s="32"/>
+      <c r="G17" s="32"/>
+    </row>
+    <row r="18" spans="1:7" ht="16" customHeight="1">
+      <c r="A18" s="32"/>
+      <c r="B18" s="32"/>
+      <c r="C18" s="32"/>
+      <c r="D18" s="32"/>
+      <c r="E18" s="32"/>
+      <c r="F18" s="32"/>
+      <c r="G18" s="32"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Address and mandatory fields: api spec, models, Keycloak single address, EmployeeService
</commit_message>
<xml_diff>
--- a/api-hub-example/example.xlsx
+++ b/api-hub-example/example.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/areddy/Downloads/employee-management-service/api-hub-example/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0D3D7D9-D4DE-274D-A61C-BE332A9D9E20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{384D9D69-3E87-2141-8FBD-3241A713E307}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="660" windowWidth="30240" windowHeight="17840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="56">
   <si>
     <t>Category</t>
   </si>
@@ -402,14 +402,13 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -419,6 +418,7 @@
     <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="API organization (organization)LockedColumnStyle" xfId="1" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
@@ -783,14 +783,14 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="17" customHeight="1">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="28"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
       <c r="G2" s="1"/>
       <c r="H2" s="3"/>
     </row>
@@ -836,7 +836,7 @@
   <dimension ref="A1:N31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" customHeight="1"/>
@@ -1081,7 +1081,9 @@
         <v>34</v>
       </c>
       <c r="B12" s="17"/>
-      <c r="C12" s="17"/>
+      <c r="C12" s="17" t="s">
+        <v>22</v>
+      </c>
       <c r="D12" s="18"/>
       <c r="E12" s="18"/>
       <c r="F12" s="10" t="s">
@@ -1305,7 +1307,9 @@
         <v>37</v>
       </c>
       <c r="B24" s="17"/>
-      <c r="C24" s="17"/>
+      <c r="C24" s="17" t="s">
+        <v>22</v>
+      </c>
       <c r="D24" s="18"/>
       <c r="E24" s="18"/>
       <c r="F24" s="10" t="s">
@@ -1590,17 +1594,17 @@
       <c r="G8" s="25"/>
     </row>
     <row r="9" spans="1:7" ht="17" customHeight="1">
-      <c r="A9" s="35" t="s">
+      <c r="A9" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="B9" s="36"/>
-      <c r="C9" s="36"/>
-      <c r="D9" s="37"/>
-      <c r="E9" s="36"/>
-      <c r="F9" s="36" t="s">
+      <c r="B9" s="35"/>
+      <c r="C9" s="35"/>
+      <c r="D9" s="36"/>
+      <c r="E9" s="35"/>
+      <c r="F9" s="35" t="s">
         <v>55</v>
       </c>
-      <c r="G9" s="38"/>
+      <c r="G9" s="37"/>
     </row>
     <row r="10" spans="1:7" ht="17" customHeight="1">
       <c r="A10" s="5"/>
@@ -1631,64 +1635,64 @@
       <c r="G11" s="4"/>
     </row>
     <row r="12" spans="1:7" ht="17" customHeight="1">
-      <c r="A12" s="29"/>
-      <c r="B12" s="30" t="s">
+      <c r="A12" s="28"/>
+      <c r="B12" s="29" t="s">
         <v>51</v>
       </c>
-      <c r="C12" s="30" t="s">
+      <c r="C12" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="D12" s="31" t="s">
+      <c r="D12" s="30" t="s">
         <v>48</v>
       </c>
-      <c r="E12" s="30"/>
-      <c r="F12" s="30"/>
-      <c r="G12" s="30"/>
+      <c r="E12" s="29"/>
+      <c r="F12" s="29"/>
+      <c r="G12" s="29"/>
     </row>
     <row r="13" spans="1:7" ht="16" customHeight="1">
-      <c r="A13" s="32"/>
-      <c r="B13" s="33" t="s">
+      <c r="A13" s="31"/>
+      <c r="B13" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="C13" s="34" t="s">
+      <c r="C13" s="33" t="s">
         <v>31</v>
       </c>
-      <c r="D13" s="34" t="s">
+      <c r="D13" s="33" t="s">
         <v>48</v>
       </c>
-      <c r="E13" s="32"/>
-      <c r="F13" s="32"/>
-      <c r="G13" s="32"/>
+      <c r="E13" s="31"/>
+      <c r="F13" s="31"/>
+      <c r="G13" s="31"/>
     </row>
     <row r="14" spans="1:7" ht="16" customHeight="1">
-      <c r="A14" s="32"/>
-      <c r="B14" s="33" t="s">
+      <c r="A14" s="31"/>
+      <c r="B14" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="C14" s="34" t="s">
+      <c r="C14" s="33" t="s">
         <v>31</v>
       </c>
-      <c r="D14" s="34" t="s">
+      <c r="D14" s="33" t="s">
         <v>48</v>
       </c>
-      <c r="E14" s="32"/>
-      <c r="F14" s="32"/>
-      <c r="G14" s="32"/>
+      <c r="E14" s="31"/>
+      <c r="F14" s="31"/>
+      <c r="G14" s="31"/>
     </row>
     <row r="15" spans="1:7" ht="16" customHeight="1">
-      <c r="A15" s="32"/>
-      <c r="B15" s="33" t="s">
+      <c r="A15" s="31"/>
+      <c r="B15" s="32" t="s">
         <v>54</v>
       </c>
-      <c r="C15" s="34" t="s">
+      <c r="C15" s="33" t="s">
         <v>31</v>
       </c>
-      <c r="D15" s="34" t="s">
+      <c r="D15" s="33" t="s">
         <v>48</v>
       </c>
-      <c r="E15" s="32"/>
-      <c r="F15" s="32"/>
-      <c r="G15" s="32"/>
+      <c r="E15" s="31"/>
+      <c r="F15" s="31"/>
+      <c r="G15" s="31"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Restore example.xlsx from stash
</commit_message>
<xml_diff>
--- a/api-hub-example/example.xlsx
+++ b/api-hub-example/example.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/areddy/Downloads/employee-management-service/api-hub-example/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57EC36BB-3F25-F14E-AB34-CEFF7E97162E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A030BA51-1C3E-3042-8A2C-DC4FEB37840A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="660" windowWidth="30240" windowHeight="17840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="660" windowWidth="30240" windowHeight="18980" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="API organization (organization)" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="56">
   <si>
     <t>Category</t>
   </si>
@@ -117,9 +117,6 @@
     <t>address</t>
   </si>
   <si>
-    <t>country</t>
-  </si>
-  <si>
     <t>String</t>
   </si>
   <si>
@@ -169,6 +166,30 @@
   </si>
   <si>
     <t>/employee</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>line1</t>
+  </si>
+  <si>
+    <t>line2</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>Zip</t>
+  </si>
+  <si>
+    <t>dto</t>
   </si>
 </sst>
 </file>
@@ -257,7 +278,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -280,6 +301,34 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -296,7 +345,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -348,6 +397,25 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="API organization (organization)LockedColumnStyle" xfId="1" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
@@ -762,10 +830,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:N31"/>
+  <dimension ref="A1:N36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12:O12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D26" sqref="D26:D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" customHeight="1"/>
@@ -833,7 +901,7 @@
         <v>24</v>
       </c>
       <c r="K2" s="27" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="L2" s="12" t="s">
         <v>25</v>
@@ -869,7 +937,9 @@
       <c r="C4" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="D4" s="4"/>
+      <c r="D4" s="4" t="s">
+        <v>48</v>
+      </c>
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
       <c r="G4" s="13"/>
@@ -887,9 +957,11 @@
         <v>30</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="D5" s="4"/>
+        <v>30</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>48</v>
+      </c>
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
       <c r="G5" s="13"/>
@@ -904,10 +976,10 @@
     <row r="6" spans="1:14" ht="17" customHeight="1">
       <c r="A6" s="5"/>
       <c r="B6" s="14" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
@@ -923,12 +995,6 @@
     </row>
     <row r="7" spans="1:14" ht="17" customHeight="1">
       <c r="A7" s="5"/>
-      <c r="B7" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="C7" s="14" t="s">
-        <v>34</v>
-      </c>
       <c r="D7" s="16"/>
       <c r="E7" s="16"/>
       <c r="F7" s="16"/>
@@ -1007,10 +1073,12 @@
     </row>
     <row r="12" spans="1:14" ht="17" customHeight="1">
       <c r="A12" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B12" s="17"/>
-      <c r="C12" s="17"/>
+      <c r="C12" s="17" t="s">
+        <v>22</v>
+      </c>
       <c r="D12" s="18"/>
       <c r="E12" s="18"/>
       <c r="F12" s="10" t="s">
@@ -1051,9 +1119,11 @@
         <v>28</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="D14" s="16"/>
+        <v>31</v>
+      </c>
+      <c r="D14" s="14" t="s">
+        <v>48</v>
+      </c>
       <c r="E14" s="16"/>
       <c r="F14" s="16"/>
       <c r="G14" s="16"/>
@@ -1068,12 +1138,14 @@
     <row r="15" spans="1:14" ht="15" customHeight="1">
       <c r="A15" s="14"/>
       <c r="B15" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="D15" s="16"/>
+        <v>31</v>
+      </c>
+      <c r="D15" s="14" t="s">
+        <v>48</v>
+      </c>
       <c r="E15" s="16"/>
       <c r="F15" s="16"/>
       <c r="G15" s="16"/>
@@ -1088,12 +1160,14 @@
     <row r="16" spans="1:14" ht="15" customHeight="1">
       <c r="A16" s="14"/>
       <c r="B16" s="14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="D16" s="16"/>
+        <v>31</v>
+      </c>
+      <c r="D16" s="14" t="s">
+        <v>48</v>
+      </c>
       <c r="E16" s="16"/>
       <c r="F16" s="16"/>
       <c r="G16" s="16"/>
@@ -1111,9 +1185,11 @@
         <v>30</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="D17" s="16"/>
+        <v>30</v>
+      </c>
+      <c r="D17" s="14" t="s">
+        <v>48</v>
+      </c>
       <c r="E17" s="16"/>
       <c r="F17" s="16"/>
       <c r="G17" s="16"/>
@@ -1127,12 +1203,8 @@
     </row>
     <row r="18" spans="1:14" ht="15" customHeight="1">
       <c r="A18" s="14"/>
-      <c r="B18" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="C18" s="14" t="s">
-        <v>32</v>
-      </c>
+      <c r="B18" s="14"/>
+      <c r="C18" s="14"/>
       <c r="D18" s="16"/>
       <c r="E18" s="16"/>
       <c r="F18" s="16"/>
@@ -1227,10 +1299,12 @@
     </row>
     <row r="24" spans="1:14" ht="17" customHeight="1">
       <c r="A24" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B24" s="17"/>
-      <c r="C24" s="17"/>
+      <c r="C24" s="17" t="s">
+        <v>22</v>
+      </c>
       <c r="D24" s="18"/>
       <c r="E24" s="18"/>
       <c r="F24" s="10" t="s">
@@ -1243,7 +1317,7 @@
         <v>24</v>
       </c>
       <c r="K24" s="27" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="L24" s="12" t="s">
         <v>25</v>
@@ -1279,7 +1353,9 @@
       <c r="C26" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="D26" s="16"/>
+      <c r="D26" s="14" t="s">
+        <v>48</v>
+      </c>
       <c r="E26" s="16"/>
       <c r="F26" s="16"/>
       <c r="G26" s="16"/>
@@ -1294,12 +1370,14 @@
     <row r="27" spans="1:14" ht="15" customHeight="1">
       <c r="A27" s="14"/>
       <c r="B27" s="14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C27" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="D27" s="16"/>
+        <v>34</v>
+      </c>
+      <c r="D27" s="14" t="s">
+        <v>48</v>
+      </c>
       <c r="E27" s="16"/>
       <c r="F27" s="16"/>
       <c r="G27" s="16"/>
@@ -1375,6 +1453,9 @@
       <c r="M31" s="15"/>
       <c r="N31" s="15"/>
     </row>
+    <row r="36" spans="3:3" ht="16" customHeight="1">
+      <c r="C36" s="29"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter alignWithMargins="0"/>
@@ -1383,9 +1464,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
@@ -1433,16 +1514,16 @@
       <c r="E2" s="22"/>
       <c r="F2" s="22"/>
       <c r="G2" s="24" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="18" customHeight="1">
       <c r="A3" s="5"/>
       <c r="B3" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>40</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>41</v>
       </c>
       <c r="D3" s="26"/>
       <c r="E3" s="4"/>
@@ -1452,10 +1533,10 @@
     <row r="4" spans="1:7" ht="18" customHeight="1">
       <c r="A4" s="5"/>
       <c r="B4" s="25" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D4" s="26"/>
       <c r="E4" s="4"/>
@@ -1465,10 +1546,10 @@
     <row r="5" spans="1:7" ht="17" customHeight="1">
       <c r="A5" s="5"/>
       <c r="B5" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D5" s="26"/>
       <c r="E5" s="4"/>
@@ -1478,10 +1559,10 @@
     <row r="6" spans="1:7" ht="17" customHeight="1">
       <c r="A6" s="5"/>
       <c r="B6" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D6" s="26"/>
       <c r="E6" s="4"/>
@@ -1491,10 +1572,10 @@
     <row r="7" spans="1:7" ht="18" customHeight="1">
       <c r="A7" s="5"/>
       <c r="B7" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>45</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>46</v>
       </c>
       <c r="D7" s="26"/>
       <c r="E7" s="4"/>
@@ -1511,40 +1592,132 @@
       <c r="G8" s="25"/>
     </row>
     <row r="9" spans="1:7" ht="17" customHeight="1">
-      <c r="A9" s="5"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="26"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="25"/>
+      <c r="A9" s="30"/>
+      <c r="B9" s="31"/>
+      <c r="C9" s="31"/>
+      <c r="D9" s="32"/>
+      <c r="E9" s="31"/>
+      <c r="F9" s="31"/>
+      <c r="G9" s="33"/>
     </row>
     <row r="10" spans="1:7" ht="17" customHeight="1">
-      <c r="A10" s="5"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="26"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
+      <c r="A10" s="34" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" s="35"/>
+      <c r="C10" s="35"/>
+      <c r="D10" s="36"/>
+      <c r="E10" s="35"/>
+      <c r="F10" s="35" t="s">
+        <v>55</v>
+      </c>
+      <c r="G10" s="35"/>
     </row>
     <row r="11" spans="1:7" ht="17" customHeight="1">
-      <c r="A11" s="5"/>
-      <c r="B11" s="25"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="26"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
+      <c r="A11" s="34"/>
+      <c r="B11" s="37" t="s">
+        <v>49</v>
+      </c>
+      <c r="C11" s="35" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" s="36" t="s">
+        <v>48</v>
+      </c>
+      <c r="E11" s="35"/>
+      <c r="F11" s="35"/>
+      <c r="G11" s="35"/>
     </row>
     <row r="12" spans="1:7" ht="17" customHeight="1">
-      <c r="A12" s="5"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="26"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
+      <c r="A12" s="34"/>
+      <c r="B12" s="35" t="s">
+        <v>50</v>
+      </c>
+      <c r="C12" s="35" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" s="36"/>
+      <c r="E12" s="35"/>
+      <c r="F12" s="35"/>
+      <c r="G12" s="35"/>
+    </row>
+    <row r="13" spans="1:7" ht="16" customHeight="1">
+      <c r="A13" s="38"/>
+      <c r="B13" s="39" t="s">
+        <v>51</v>
+      </c>
+      <c r="C13" s="39" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13" s="39" t="s">
+        <v>48</v>
+      </c>
+      <c r="E13" s="38"/>
+      <c r="F13" s="38"/>
+      <c r="G13" s="38"/>
+    </row>
+    <row r="14" spans="1:7" ht="16" customHeight="1">
+      <c r="A14" s="38"/>
+      <c r="B14" s="39" t="s">
+        <v>52</v>
+      </c>
+      <c r="C14" s="39" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" s="39" t="s">
+        <v>48</v>
+      </c>
+      <c r="E14" s="38"/>
+      <c r="F14" s="38"/>
+      <c r="G14" s="38"/>
+    </row>
+    <row r="15" spans="1:7" ht="16" customHeight="1">
+      <c r="A15" s="38"/>
+      <c r="B15" s="39" t="s">
+        <v>54</v>
+      </c>
+      <c r="C15" s="39" t="s">
+        <v>31</v>
+      </c>
+      <c r="D15" s="39" t="s">
+        <v>48</v>
+      </c>
+      <c r="E15" s="38"/>
+      <c r="F15" s="38"/>
+      <c r="G15" s="38"/>
+    </row>
+    <row r="16" spans="1:7" ht="16" customHeight="1">
+      <c r="A16" s="38"/>
+      <c r="B16" s="39" t="s">
+        <v>53</v>
+      </c>
+      <c r="C16" s="39" t="s">
+        <v>31</v>
+      </c>
+      <c r="D16" s="39" t="s">
+        <v>48</v>
+      </c>
+      <c r="E16" s="38"/>
+      <c r="F16" s="38"/>
+      <c r="G16" s="38"/>
+    </row>
+    <row r="17" spans="1:7" ht="16" customHeight="1">
+      <c r="A17" s="38"/>
+      <c r="B17" s="38"/>
+      <c r="C17" s="38"/>
+      <c r="D17" s="38"/>
+      <c r="E17" s="38"/>
+      <c r="F17" s="38"/>
+      <c r="G17" s="38"/>
+    </row>
+    <row r="18" spans="1:7" ht="16" customHeight="1">
+      <c r="A18" s="38"/>
+      <c r="B18" s="38"/>
+      <c r="C18" s="38"/>
+      <c r="D18" s="38"/>
+      <c r="E18" s="38"/>
+      <c r="F18" s="38"/>
+      <c r="G18" s="38"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>